<commit_message>
Change image sizes and add AC
</commit_message>
<xml_diff>
--- a/Dialog-content/code/srcs/Effet_Core_Mecanics.xlsx
+++ b/Dialog-content/code/srcs/Effet_Core_Mecanics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clarisse/Documents/MSE/Fall_2023/GT/Projet/Eco-logis/Dialog-content/code/srcs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC356C92-9347-BD4A-A3CF-EC6AD6CB2991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD06A73-BEFB-A341-B285-9266D645F69A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="880" windowWidth="35240" windowHeight="22500" activeTab="4" xr2:uid="{7A2FE946-C167-4F95-B414-ADE868C81E0F}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="178">
   <si>
     <t>Bonheur</t>
   </si>
@@ -537,12 +537,6 @@
     <t>PlayStation Blue-Ray</t>
   </si>
   <si>
-    <t>G (1)</t>
-  </si>
-  <si>
-    <t>F (1)</t>
-  </si>
-  <si>
     <t>G</t>
   </si>
   <si>
@@ -577,6 +571,9 @@
   </si>
   <si>
     <t>tv</t>
+  </si>
+  <si>
+    <t>air_conditioner</t>
   </si>
 </sst>
 </file>
@@ -887,8 +884,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CB7712E9-F7B8-7D4E-9E05-1FD32722E9CD}" name="IMPACT_DET" displayName="IMPACT_DET" ref="A1:I46" totalsRowShown="0">
   <autoFilter ref="A1:I46" xr:uid="{CB7712E9-F7B8-7D4E-9E05-1FD32722E9CD}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A21:I24">
-    <sortCondition ref="G1:G46"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I46">
+    <sortCondition ref="A1:A46"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{63E7E744-D15E-5040-BC35-D692B7183853}" name="Objet"/>
@@ -4299,10 +4296,10 @@
   <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView zoomScale="159" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4350,34 +4347,34 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="C2">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="G2" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>2.4</v>
+        <v>225</v>
       </c>
       <c r="H2" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
-        <v>9.6000000000000014</v>
+        <v>40</v>
       </c>
       <c r="I2" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 2, FALSE) *IMPACT_DET[[#This Row],[Finance (mult)]]</f>
-        <v>8.4</v>
+        <v>0</v>
       </c>
       <c r="K2" s="16" t="s">
         <v>139</v>
@@ -4385,34 +4382,31 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B3" t="s">
-        <v>101</v>
+        <v>172</v>
       </c>
       <c r="C3">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="G3" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>3.2</v>
+        <v>41</v>
       </c>
       <c r="H3" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
-        <v>10.8</v>
+        <v>5</v>
       </c>
       <c r="I3" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 2, FALSE) *IMPACT_DET[[#This Row],[Finance (mult)]]</f>
-        <v>7.7000000000000011</v>
+        <v>0</v>
       </c>
       <c r="K3" s="17" t="s">
         <v>140</v>
@@ -4420,74 +4414,74 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="G4" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>4</v>
+        <v>2.4</v>
       </c>
       <c r="H4" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
-        <v>12</v>
+        <v>9.6000000000000014</v>
       </c>
       <c r="I4" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 2, FALSE) *IMPACT_DET[[#This Row],[Finance (mult)]]</f>
-        <v>7</v>
+        <v>8.4</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>173</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G5" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>1.18</v>
+        <v>3.2</v>
       </c>
       <c r="H5" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
-        <v>50</v>
+        <v>10.8</v>
       </c>
       <c r="I5" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 2, FALSE) *IMPACT_DET[[#This Row],[Finance (mult)]]</f>
-        <v>0</v>
+        <v>7.7000000000000011</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>173</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -4503,23 +4497,23 @@
       </c>
       <c r="G6" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>12.9</v>
+        <v>4</v>
       </c>
       <c r="H6" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="I6" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 2, FALSE) *IMPACT_DET[[#This Row],[Finance (mult)]]</f>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -4535,7 +4529,7 @@
       </c>
       <c r="G7" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>0.88</v>
+        <v>1.18</v>
       </c>
       <c r="H7" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
@@ -4548,10 +4542,10 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>81</v>
+        <v>142</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -4567,180 +4561,180 @@
       </c>
       <c r="G8" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>2</v>
+        <v>12.9</v>
       </c>
       <c r="H8" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="I8" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 2, FALSE) *IMPACT_DET[[#This Row],[Finance (mult)]]</f>
-        <v>1265</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>143</v>
       </c>
       <c r="B9" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C9">
-        <v>1.65</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>1.65</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>1.65</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G9" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>3.3</v>
+        <v>0.88</v>
       </c>
       <c r="H9" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
-        <v>8.25</v>
+        <v>50</v>
       </c>
       <c r="I9" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 2, FALSE) *IMPACT_DET[[#This Row],[Finance (mult)]]</f>
-        <v>632.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>177</v>
       </c>
       <c r="B10" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C10">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="F10">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="G10" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H10" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
-        <v>12.5</v>
+        <v>5</v>
       </c>
       <c r="I10" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 2, FALSE) *IMPACT_DET[[#This Row],[Finance (mult)]]</f>
-        <v>379.5</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>102</v>
+        <v>177</v>
       </c>
       <c r="B11" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>1.65</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>1.65</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>1.65</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G11" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>1.23</v>
+        <v>3.3</v>
       </c>
       <c r="H11" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
-        <v>20</v>
+        <v>8.25</v>
       </c>
       <c r="I11" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 2, FALSE) *IMPACT_DET[[#This Row],[Finance (mult)]]</f>
-        <v>2350</v>
+        <v>632.5</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>102</v>
+        <v>177</v>
       </c>
       <c r="B12" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C12">
-        <v>1.9</v>
+        <v>2.5</v>
       </c>
       <c r="D12">
-        <v>1.2</v>
+        <v>2.5</v>
       </c>
       <c r="E12">
-        <v>1.9</v>
+        <v>2.5</v>
       </c>
       <c r="F12">
-        <v>2</v>
+        <v>0.3</v>
       </c>
       <c r="G12" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>2.3369999999999997</v>
+        <v>5</v>
       </c>
       <c r="H12" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
-        <v>38</v>
+        <v>12.5</v>
       </c>
       <c r="I12" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 2, FALSE) *IMPACT_DET[[#This Row],[Finance (mult)]]</f>
-        <v>4700</v>
+        <v>379.5</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>102</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>86</v>
+        <v>53</v>
       </c>
       <c r="C13">
-        <v>2.2999999999999998</v>
+        <v>1</v>
       </c>
       <c r="D13">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>2.2999999999999998</v>
+        <v>1</v>
       </c>
       <c r="F13">
-        <v>2.1</v>
+        <v>1</v>
       </c>
       <c r="G13" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>2.8289999999999997</v>
+        <v>47.5</v>
       </c>
       <c r="H13" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="I13" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 2, FALSE) *IMPACT_DET[[#This Row],[Finance (mult)]]</f>
-        <v>4935</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>144</v>
+        <v>102</v>
       </c>
       <c r="B14" t="s">
         <v>88</v>
@@ -4759,215 +4753,215 @@
       </c>
       <c r="G14" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>40</v>
+        <v>1.23</v>
       </c>
       <c r="H14" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="I14" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 2, FALSE) *IMPACT_DET[[#This Row],[Finance (mult)]]</f>
-        <v>1899</v>
+        <v>2350</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>144</v>
+        <v>102</v>
       </c>
       <c r="B15" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C15">
-        <v>1.125</v>
+        <v>1.9</v>
       </c>
       <c r="D15">
-        <v>1.4</v>
+        <v>1.2</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>1.9</v>
       </c>
       <c r="F15">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="G15" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>45</v>
+        <v>2.3369999999999997</v>
       </c>
       <c r="H15" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
-        <v>38.400000000000006</v>
+        <v>38</v>
       </c>
       <c r="I15" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 2, FALSE) *IMPACT_DET[[#This Row],[Finance (mult)]]</f>
-        <v>1329.3</v>
+        <v>4700</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>144</v>
+        <v>102</v>
       </c>
       <c r="B16" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C16">
-        <v>1.25</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D16">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F16">
-        <v>0.5</v>
+        <v>2.1</v>
       </c>
       <c r="G16" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>50</v>
+        <v>2.8289999999999997</v>
       </c>
       <c r="H16" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
-        <v>29.599999999999994</v>
+        <v>46</v>
       </c>
       <c r="I16" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 2, FALSE) *IMPACT_DET[[#This Row],[Finance (mult)]]</f>
-        <v>949.5</v>
+        <v>4935</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>125</v>
+        <v>174</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C17">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="D17">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G17" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>33.6</v>
+        <v>138</v>
       </c>
       <c r="H17" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
-        <v>40.799999999999997</v>
+        <v>4</v>
       </c>
       <c r="I17" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 2, FALSE) *IMPACT_DET[[#This Row],[Finance (mult)]]</f>
-        <v>1950</v>
+        <v>619</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>125</v>
+        <v>174</v>
       </c>
       <c r="B18" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C18">
-        <v>0.65</v>
+        <v>1.5</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="E18">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="F18">
-        <v>2</v>
+        <v>1.2</v>
       </c>
       <c r="G18" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>54.6</v>
+        <v>207</v>
       </c>
       <c r="H18" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
-        <v>32</v>
+        <v>3.3999999999999986</v>
       </c>
       <c r="I18" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 2, FALSE) *IMPACT_DET[[#This Row],[Finance (mult)]]</f>
-        <v>1300</v>
+        <v>742.8</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>174</v>
       </c>
       <c r="B19" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="C19">
-        <v>0.89</v>
+        <v>1.7</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>0.97</v>
       </c>
       <c r="E19">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>1.03</v>
       </c>
       <c r="G19" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>74.760000000000005</v>
+        <v>234.6</v>
       </c>
       <c r="H19" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
-        <v>41.5</v>
+        <v>3.8800000000000026</v>
       </c>
       <c r="I19" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 2, FALSE) *IMPACT_DET[[#This Row],[Finance (mult)]]</f>
-        <v>650</v>
+        <v>637.57000000000005</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>125</v>
+        <v>174</v>
       </c>
       <c r="B20" t="s">
-        <v>91</v>
+        <v>145</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>2.6</v>
       </c>
       <c r="G20" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>84</v>
+        <v>345</v>
       </c>
       <c r="H20" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
-        <v>51</v>
+        <v>3.6000000000000014</v>
       </c>
       <c r="I20" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 2, FALSE) *IMPACT_DET[[#This Row],[Finance (mult)]]</f>
-        <v>650</v>
+        <v>1609.4</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>176</v>
+        <v>144</v>
       </c>
       <c r="B21" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -4983,189 +4977,189 @@
       </c>
       <c r="G21" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>138</v>
+        <v>40</v>
       </c>
       <c r="H21" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="I21" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 2, FALSE) *IMPACT_DET[[#This Row],[Finance (mult)]]</f>
-        <v>619</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>176</v>
+        <v>144</v>
       </c>
       <c r="B22" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="C22">
-        <v>1.5</v>
+        <v>1.125</v>
       </c>
       <c r="D22">
-        <v>0.85</v>
+        <v>1.4</v>
       </c>
       <c r="E22">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="F22">
-        <v>1.2</v>
+        <v>0.7</v>
       </c>
       <c r="G22" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>207</v>
+        <v>45</v>
       </c>
       <c r="H22" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
-        <v>3.3999999999999986</v>
+        <v>38.400000000000006</v>
       </c>
       <c r="I22" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 2, FALSE) *IMPACT_DET[[#This Row],[Finance (mult)]]</f>
-        <v>742.8</v>
+        <v>1329.3</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>176</v>
+        <v>144</v>
       </c>
       <c r="B23" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="C23">
-        <v>1.7</v>
+        <v>1.25</v>
       </c>
       <c r="D23">
-        <v>0.97</v>
+        <v>1.6</v>
       </c>
       <c r="E23">
-        <v>0.97</v>
+        <v>1</v>
       </c>
       <c r="F23">
-        <v>1.03</v>
+        <v>0.5</v>
       </c>
       <c r="G23" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>234.6</v>
+        <v>50</v>
       </c>
       <c r="H23" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
-        <v>3.8800000000000026</v>
+        <v>29.599999999999994</v>
       </c>
       <c r="I23" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 2, FALSE) *IMPACT_DET[[#This Row],[Finance (mult)]]</f>
-        <v>637.57000000000005</v>
+        <v>949.5</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>176</v>
+        <v>125</v>
       </c>
       <c r="B24" t="s">
-        <v>145</v>
+        <v>88</v>
       </c>
       <c r="C24">
-        <v>2.5</v>
+        <v>0.4</v>
       </c>
       <c r="D24">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="E24">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="F24">
-        <v>2.6</v>
+        <v>3</v>
       </c>
       <c r="G24" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>345</v>
+        <v>33.6</v>
       </c>
       <c r="H24" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
-        <v>3.6000000000000014</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="I24" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 2, FALSE) *IMPACT_DET[[#This Row],[Finance (mult)]]</f>
-        <v>1609.4</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>101</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>0.65</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G25" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>40</v>
+        <v>54.6</v>
       </c>
       <c r="H25" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="I25" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 2, FALSE) *IMPACT_DET[[#This Row],[Finance (mult)]]</f>
-        <v>0</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>125</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>0.89</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="F26">
         <v>1</v>
       </c>
       <c r="G26" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>47.5</v>
+        <v>74.760000000000005</v>
       </c>
       <c r="H26" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
-        <v>30</v>
+        <v>41.5</v>
       </c>
       <c r="I26" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 2, FALSE) *IMPACT_DET[[#This Row],[Finance (mult)]]</f>
-        <v>0</v>
+        <v>650</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>125</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -5175,15 +5169,15 @@
       </c>
       <c r="G27" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>225</v>
+        <v>84</v>
       </c>
       <c r="H27" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="I27" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 2, FALSE) *IMPACT_DET[[#This Row],[Finance (mult)]]</f>
-        <v>0</v>
+        <v>650</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -5220,7 +5214,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B29" t="s">
         <v>53</v>
@@ -5348,7 +5342,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B33" t="s">
         <v>161</v>
@@ -5367,7 +5361,7 @@
       </c>
       <c r="G33" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>209.8</v>
+        <v>55.7</v>
       </c>
       <c r="H33" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
@@ -5380,13 +5374,13 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B34" t="s">
         <v>162</v>
       </c>
       <c r="C34">
-        <v>1.05</v>
+        <v>1.45</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -5399,7 +5393,7 @@
       </c>
       <c r="G34" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>220.29000000000002</v>
+        <v>80.765000000000001</v>
       </c>
       <c r="H34" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
@@ -5412,7 +5406,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B35" t="s">
         <v>161</v>
@@ -5431,7 +5425,7 @@
       </c>
       <c r="G35" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>55.7</v>
+        <v>209.8</v>
       </c>
       <c r="H35" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
@@ -5444,13 +5438,13 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B36" t="s">
         <v>162</v>
       </c>
       <c r="C36">
-        <v>1.45</v>
+        <v>1.05</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -5463,7 +5457,7 @@
       </c>
       <c r="G36" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>80.765000000000001</v>
+        <v>220.29000000000002</v>
       </c>
       <c r="H36" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
@@ -5476,10 +5470,10 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B37" t="s">
-        <v>166</v>
+        <v>91</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -5508,10 +5502,10 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B38" t="s">
-        <v>145</v>
+        <v>111</v>
       </c>
       <c r="C38">
         <v>1.25</v>
@@ -5540,10 +5534,10 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B39" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="C39">
         <v>2.4</v>
@@ -5572,10 +5566,10 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B40" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C40">
         <v>2.4</v>
@@ -5604,30 +5598,30 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
       <c r="B41" t="s">
-        <v>169</v>
+        <v>53</v>
       </c>
       <c r="C41">
         <v>1</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E41">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F41">
         <v>1</v>
       </c>
       <c r="G41" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>4.5250000000000004</v>
+        <v>40</v>
       </c>
       <c r="H41" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="I41" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 2, FALSE) *IMPACT_DET[[#This Row],[Finance (mult)]]</f>
@@ -5636,30 +5630,30 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B42" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C42">
-        <v>0.5</v>
+        <v>0.01</v>
       </c>
       <c r="D42">
         <v>1</v>
       </c>
       <c r="E42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F42">
         <v>1</v>
       </c>
       <c r="G42" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>2.2625000000000002</v>
+        <v>4.5250000000000005E-2</v>
       </c>
       <c r="H42" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
-        <v>19</v>
+        <v>-1</v>
       </c>
       <c r="I42" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 2, FALSE) *IMPACT_DET[[#This Row],[Finance (mult)]]</f>
@@ -5668,13 +5662,13 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B43" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C43">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -5687,7 +5681,7 @@
       </c>
       <c r="G43" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>2.2625000000000002</v>
+        <v>0.22625000000000003</v>
       </c>
       <c r="H43" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
@@ -5700,30 +5694,30 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>166</v>
+      </c>
+      <c r="B44" t="s">
         <v>168</v>
       </c>
-      <c r="B44" t="s">
-        <v>172</v>
-      </c>
       <c r="C44">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
       <c r="E44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F44">
         <v>1</v>
       </c>
       <c r="G44" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>0.22625000000000003</v>
+        <v>2.2625000000000002</v>
       </c>
       <c r="H44" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="I44" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 2, FALSE) *IMPACT_DET[[#This Row],[Finance (mult)]]</f>
@@ -5732,30 +5726,30 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B45" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C45">
-        <v>0.01</v>
+        <v>0.5</v>
       </c>
       <c r="D45">
         <v>1</v>
       </c>
       <c r="E45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F45">
         <v>1</v>
       </c>
       <c r="G45" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>4.5250000000000005E-2</v>
+        <v>2.2625000000000002</v>
       </c>
       <c r="H45" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="I45" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 2, FALSE) *IMPACT_DET[[#This Row],[Finance (mult)]]</f>
@@ -5764,7 +5758,10 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>174</v>
+        <v>166</v>
+      </c>
+      <c r="B46" t="s">
+        <v>167</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -5773,18 +5770,18 @@
         <v>1</v>
       </c>
       <c r="E46">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F46">
         <v>1</v>
       </c>
       <c r="G46" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 3, FALSE) *IMPACT_DET[[#This Row],[Energie (mult)]]</f>
-        <v>41</v>
+        <v>4.5250000000000004</v>
       </c>
       <c r="H46" s="17">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 5, FALSE) *IMPACT_DET[[#This Row],[Bien-être + (db) (mult)]] - VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 4, FALSE) *IMPACT_DET[[#This Row],[Bien-être - (db) (mult)]]</f>
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="I46" s="16">
         <f>VLOOKUP(IMPACT_DET[[#This Row],[Objet]], BASIC_VALUES[], 2, FALSE) *IMPACT_DET[[#This Row],[Finance (mult)]]</f>
@@ -5807,7 +5804,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J15" sqref="J15"/>
+      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5863,7 +5860,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B3">
         <v>7</v>
@@ -5880,7 +5877,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>177</v>
       </c>
       <c r="B4">
         <v>1265</v>
@@ -5931,7 +5928,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B7">
         <v>619</v>
@@ -6055,7 +6052,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C15">
         <v>148</v>
@@ -6120,7 +6117,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B19">
         <v>449.9</v>
@@ -6137,7 +6134,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C20">
         <v>4.5250000000000004</v>
@@ -6154,7 +6151,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C21">
         <v>41</v>

</xml_diff>